<commit_message>
feat: aprimorar filtros de eventos e calendário acadêmico
- Atualiza o filtro de eventos para incluir eventos gerais (courseId null) além de eventos específicos.
- Adiciona filtro padrão para exibir apenas eventos do último mês em diante.
- Melhora a busca de horários normalizando o nome das salas e implementando busca por termos.
- Adiciona suporte para importar eventos com a opção de não associar a um curso específico.
- Implementa parsing de datas em formato brasileiro para o calendário acadêmico.
- Atualiza o template de eventos.
</commit_message>
<xml_diff>
--- a/templates/planilha_modelo_eventos.xlsx
+++ b/templates/planilha_modelo_eventos.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29518"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29602"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F35C92FF-50DB-4064-80B6-03A94689A1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{103C7367-D23D-4EF4-863B-B05F0AC4D9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>titulo</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>nome_curso</t>
+  </si>
+  <si>
+    <t>link</t>
   </si>
   <si>
     <t>Administração</t>
@@ -185,9 +188,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{517370BD-1B9E-4FE0-B0E4-B5FE0F09CCF0}" name="Tabela1" displayName="Tabela1" ref="A1:G2" totalsRowShown="0">
-  <autoFilter ref="A1:G2" xr:uid="{517370BD-1B9E-4FE0-B0E4-B5FE0F09CCF0}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{517370BD-1B9E-4FE0-B0E4-B5FE0F09CCF0}" name="Tabela1" displayName="Tabela1" ref="A1:H15" totalsRowShown="0">
+  <autoFilter ref="A1:H15" xr:uid="{517370BD-1B9E-4FE0-B0E4-B5FE0F09CCF0}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{16724F5A-F452-4D71-A970-C60861029601}" name="titulo"/>
     <tableColumn id="2" xr3:uid="{A320B899-6C1E-49AA-AD00-FD171B94F19E}" name="descricao"/>
     <tableColumn id="3" xr3:uid="{FAE65FAA-6D11-47F0-A774-BE1EC1E61556}" name="data_inicio" dataDxfId="1"/>
@@ -195,6 +198,7 @@
     <tableColumn id="5" xr3:uid="{96A51BCB-B00D-4201-90A7-9786A1E9C412}" name="local"/>
     <tableColumn id="6" xr3:uid="{501B313D-7E4A-4C11-AED1-899A5B24F7A6}" name="tipo"/>
     <tableColumn id="7" xr3:uid="{14DDF4EE-1E0F-4B5A-86CD-966D03F4F799}" name="nome_curso"/>
+    <tableColumn id="8" xr3:uid="{027DD627-4BAC-4C3E-A8DF-2B36F3DD7F63}" name="link"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -485,7 +489,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
@@ -500,7 +504,7 @@
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,6 +525,9 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -558,117 +565,117 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>